<commit_message>
Export Excel & Perbaikan
- Export Excel Anggota
- Export Ecel Pegawai
- Menghilangkan button detail di fitur lihat pinjman
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>NAMA</t>
   </si>
@@ -29,25 +29,22 @@
     <t>ALAMAT</t>
   </si>
   <si>
-    <t xml:space="preserve">Gunawan Asmeda </t>
-  </si>
-  <si>
-    <t>Jl Durian Runtuh No 16, Lamongan</t>
-  </si>
-  <si>
-    <t>Andika Nanda</t>
-  </si>
-  <si>
-    <t>Lamongan Jawa Timur</t>
-  </si>
-  <si>
-    <t>Anriko Chiesa</t>
-  </si>
-  <si>
     <t>NIK</t>
   </si>
   <si>
+    <t>Agus Budi</t>
+  </si>
+  <si>
+    <t>Aurel Herman</t>
+  </si>
+  <si>
     <t>NO HP</t>
+  </si>
+  <si>
+    <t>Lamongan</t>
+  </si>
+  <si>
+    <t>Jember</t>
   </si>
 </sst>
 </file>
@@ -389,24 +386,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="63.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -415,54 +411,39 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1424001</v>
+        <v>14241010994</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>81253709129</v>
+        <v>81777888999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1424002</v>
+        <v>14241010123</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>81456789098</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1424003</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>81878788698</v>
+        <v>81625827019</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>